<commit_message>
Update Dataset and Transformers File
</commit_message>
<xml_diff>
--- a/data/2025/political-classification-model-videos.xlsx
+++ b/data/2025/political-classification-model-videos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\isss1\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CA876207-2811-4A49-9929-F5B670FB08BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EEE9DEF-ED33-43CA-8D87-E924818654D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{156379FD-5550-4272-9C5F-CA1190519004}"/>
+    <workbookView xWindow="3465" yWindow="3465" windowWidth="21600" windowHeight="11295" xr2:uid="{156379FD-5550-4272-9C5F-CA1190519004}"/>
   </bookViews>
   <sheets>
     <sheet name="dataset" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="43">
   <si>
     <t>party</t>
   </si>
@@ -114,6 +114,57 @@
   </si>
   <si>
     <t>https://www.youtube.com/watch?v=kBslXtLPr30</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=X1sNH8kuV6A</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=wcuU-MQVOQE</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=t1UNkoMef44</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=1GHrpFNOmvo</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=MuXdxsY8p6s</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=V9tf4dbJfB4</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=DQwllYSHoTE</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=y5qdzzAdoIQ</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=QD_8skxLiJs</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=e4WpbJ6xn40</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=tNDy7e37KrI</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=92QvS2E3TxY</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=cQsXLCVEq3U</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=qw_jOklPaDs</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=1Yt0epYn71I</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=fe4NzX_h3tY</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=yf7d_5wGAIM</t>
   </si>
 </sst>
 </file>
@@ -496,10 +547,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B56655D-DCB3-467B-BAB3-152388186686}">
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:B39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="I35" sqref="I35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -670,6 +721,150 @@
       </c>
       <c r="B21" s="1" t="s">
         <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>2</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>2</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>8</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>2</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>2</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>2</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>2</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>2</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>2</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>2</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>9</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>9</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>9</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>9</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>9</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>9</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>8</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>8</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -690,6 +885,24 @@
     <hyperlink ref="B19" r:id="rId14" xr:uid="{71A40883-9808-496B-8E36-57DA0BD20F4A}"/>
     <hyperlink ref="B20" r:id="rId15" xr:uid="{73EF2D65-4F1A-41D0-B161-B1B6DAF7F2C4}"/>
     <hyperlink ref="B21" r:id="rId16" xr:uid="{48D931D8-528F-45AD-B1F2-47AD0794752B}"/>
+    <hyperlink ref="B22" r:id="rId17" xr:uid="{E6EA951A-B86D-4D32-9BCF-8BB2C857B774}"/>
+    <hyperlink ref="B23" r:id="rId18" xr:uid="{8866CF15-DD49-4F71-9EBD-D803E8867D67}"/>
+    <hyperlink ref="B24" r:id="rId19" xr:uid="{1BB2C589-BE4E-4C45-B274-0C8E29ED98A2}"/>
+    <hyperlink ref="B25" r:id="rId20" xr:uid="{8D2D1496-80FD-425D-864B-4F9318AE35C2}"/>
+    <hyperlink ref="B26" r:id="rId21" xr:uid="{177FB095-A768-4C4D-A990-6B48BF141A2F}"/>
+    <hyperlink ref="B27" r:id="rId22" xr:uid="{5E3E9AD2-9C0F-47F0-BCF0-CEEBF7E56CC8}"/>
+    <hyperlink ref="B28" r:id="rId23" xr:uid="{3E73F305-5620-4DAC-AAB6-F77B2C8565B6}"/>
+    <hyperlink ref="B29" r:id="rId24" xr:uid="{BA6DADBD-57BD-4BE0-8D57-ADF2444FD2C8}"/>
+    <hyperlink ref="B30" r:id="rId25" xr:uid="{10FDF6C9-260C-4828-A381-2C6151879861}"/>
+    <hyperlink ref="B31" r:id="rId26" xr:uid="{6FC2FBAF-9F01-4E06-99B8-2006744C17DE}"/>
+    <hyperlink ref="B32" r:id="rId27" xr:uid="{5E0B4320-2ECA-470C-9FA8-03A0FFC16726}"/>
+    <hyperlink ref="B33" r:id="rId28" xr:uid="{7AE279D2-D550-429D-B711-47E2334DF6EB}"/>
+    <hyperlink ref="B34" r:id="rId29" xr:uid="{5164C490-05F9-42F9-BB37-5EAE2BE3AA31}"/>
+    <hyperlink ref="B35" r:id="rId30" xr:uid="{30960D3D-3746-4F81-8382-8A6D2B8283BD}"/>
+    <hyperlink ref="B36" r:id="rId31" xr:uid="{E70BF7B4-E63A-4C71-8940-57C20AA79BD9}"/>
+    <hyperlink ref="B37" r:id="rId32" xr:uid="{77708FE6-EC6C-48BF-A513-5923DFA1F623}"/>
+    <hyperlink ref="B38" r:id="rId33" xr:uid="{A689ED14-DB87-41B0-81DB-388ECF6E11B6}"/>
+    <hyperlink ref="B39" r:id="rId34" xr:uid="{4B1209F2-3DC9-46E3-BA51-692E20CE12DA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>